<commit_message>
added show password, angkatan on Register / Create Account
</commit_message>
<xml_diff>
--- a/assets/template/Mahasiswa-Template.xlsx
+++ b/assets/template/Mahasiswa-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trisna Nugraha\Documents\Surat-STIK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\surat-stik\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1921DA14-F809-4D7A-9E8D-B98756F0A95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B125BB15-5640-4057-95EE-E3FA4A7B006A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{6F95BCFC-FFB5-4753-8B33-10B0D2A5EAB9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6F95BCFC-FFB5-4753-8B33-10B0D2A5EAB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nama Mahasiswa</t>
   </si>
@@ -44,17 +44,35 @@
     <t>Sindikat</t>
   </si>
   <si>
-    <t>Trisna Nugraha</t>
-  </si>
-  <si>
     <t>Sindikat I</t>
+  </si>
+  <si>
+    <t>Alamat</t>
+  </si>
+  <si>
+    <t>No. HP</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Jalan Maju Merdeka</t>
+  </si>
+  <si>
+    <t>08123456789</t>
+  </si>
+  <si>
+    <t>Angkatan</t>
+  </si>
+  <si>
+    <t>79/WTP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,16 +80,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -79,12 +111,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,41 +458,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445A880E-2BA3-4B45-A49C-02009C0BE021}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>123</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>